<commit_message>
Finalize QA pass: root docs sync, figure refresh, registry updates
</commit_message>
<xml_diff>
--- a/_figures/figures_data.xlsx
+++ b/_figures/figures_data.xlsx
@@ -11634,7 +11634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11648,82 +11648,149 @@
     <row r="1">
       <c r="A1" s="5" t="inlineStr">
         <is>
-          <t>Regulatory Landscape Comparison: US vs EU</t>
+          <t>Regulatory Landscape Comparison: US vs EU vs UK vs China</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>United States (US)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>European Union (EU)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>United Kingdom (UK)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>China</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Feature</t>
+          <t>Nutraceutical Definition</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>United States (US)</t>
+          <t>Undefined (Food vs Drug)</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>European Union (EU)</t>
+          <t>Undefined (Feed vs VMP)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Undefined (Feed vs VMP)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Undefined (Feed Additive vs VMP)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Nutraceutical Definition</t>
+          <t>Regulatory Body</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Undefined (Food vs Drug)</t>
+          <t>FDA-CVM &amp; AAFCO</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Undefined (Feed vs VMP)</t>
+          <t>EFSA &amp; National Agencies</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>VMD &amp; FSA</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>MARA &amp; SAMR</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Regulatory Body</t>
+          <t>Disease Claims</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>FDA-CVM &amp; AAFCO</t>
+          <t>Prohibited (Drug only)</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>EFSA &amp; National Agencies</t>
+          <t>Prohibited (PARNUTs exception)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Prohibited (Drug only)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Restricted by registration class</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Disease Claims</t>
+          <t>Market Entry Speed</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Prohibited (Drug only)</t>
+          <t>Fast (Notification)</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Prohibited (PARNUTs exception)</t>
+          <t>Slow (Dossier Approval)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Medium (Route-dependent)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Medium-Slow (Registration dependent)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Market Entry Speed</t>
+          <t>Source: FDA-CVM, EFSA, UK VMD/FSA, MARA filings.</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -11737,6 +11804,7 @@
         </is>
       </c>
     </row>
+    <row r="8"/>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
@@ -11744,6 +11812,16 @@
         </is>
       </c>
     </row>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13543,7 +13621,14 @@
     <row r="1">
       <c r="A1" s="5" t="inlineStr">
         <is>
-          <t>Growth of the Senior Pet Wellness Market</t>
+          <t>Pharma Integration Funnel (Relative Integration Potential)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Relative Integration Potential (Index, Trial = 100)</t>
         </is>
       </c>
     </row>
@@ -13576,8 +13661,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>2030</v>
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Source: Internal funnel model calibrated with S115 and S116 portfolio pathways.</t>
+        </is>
       </c>
       <c r="B6" s="3" t="n">
         <v>20</v>
@@ -14756,7 +14843,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -15298,7 +15384,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Aker BioMarine</t>
+          <t>Source: Annual Reports/Filing Data (S115, S117, S118, S119, S120), Master Model (S089), Transaction Context (S125).</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
@@ -15409,7 +15495,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Brand Loyalty</t>
+          <t>Source: Internal strategy normalization over S089 value pools and benchmark assumptions.</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">

</xml_diff>

<commit_message>
Fix whitepaper regression issues
</commit_message>
<xml_diff>
--- a/_figures/figures_data.xlsx
+++ b/_figures/figures_data.xlsx
@@ -59,6 +59,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DOCX_TABLE_SYNC" sheetId="51" state="visible" r:id="rId51"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DOCX_FIGURE_HARMONIZATION" sheetId="52" state="visible" r:id="rId52"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 50" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure Cattle Inventory" sheetId="54" state="visible" r:id="rId54"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -2703,7 +2704,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -4419,7 +4420,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -4546,7 +4547,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -6986,7 +6987,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -13230,7 +13231,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13248,7 +13249,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -13378,7 +13378,6 @@
         <v>89.5</v>
       </c>
     </row>
-    <row r="10"/>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
@@ -13386,24 +13385,6 @@
         </is>
       </c>
     </row>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -13983,7 +13964,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14001,7 +13982,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -14097,7 +14077,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8"/>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
@@ -14105,26 +14084,6 @@
         </is>
       </c>
     </row>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -20011,6 +19970,321 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Global Cattle Inventory: The Western Contraction</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>LATAM_scaled</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>India_scaled</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B4" t="n">
+        <v>95</v>
+      </c>
+      <c r="C4" t="n">
+        <v>78</v>
+      </c>
+      <c r="D4" t="n">
+        <v>35</v>
+      </c>
+      <c r="E4" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B5" t="n">
+        <v>94.44285714285715</v>
+      </c>
+      <c r="C5" t="n">
+        <v>77.57142857142857</v>
+      </c>
+      <c r="D5" t="n">
+        <v>35.10714285714285</v>
+      </c>
+      <c r="E5" t="n">
+        <v>19.03571428571428</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B6" t="n">
+        <v>93.88571428571429</v>
+      </c>
+      <c r="C6" t="n">
+        <v>77.14285714285714</v>
+      </c>
+      <c r="D6" t="n">
+        <v>35.21428571428572</v>
+      </c>
+      <c r="E6" t="n">
+        <v>19.07142857142857</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B7" t="n">
+        <v>93.32857142857142</v>
+      </c>
+      <c r="C7" t="n">
+        <v>76.71428571428571</v>
+      </c>
+      <c r="D7" t="n">
+        <v>35.32142857142857</v>
+      </c>
+      <c r="E7" t="n">
+        <v>19.10714285714286</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B8" t="n">
+        <v>92.77142857142857</v>
+      </c>
+      <c r="C8" t="n">
+        <v>76.28571428571429</v>
+      </c>
+      <c r="D8" t="n">
+        <v>35.42857142857143</v>
+      </c>
+      <c r="E8" t="n">
+        <v>19.14285714285714</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B9" t="n">
+        <v>92.21428571428572</v>
+      </c>
+      <c r="C9" t="n">
+        <v>75.85714285714286</v>
+      </c>
+      <c r="D9" t="n">
+        <v>35.53571428571428</v>
+      </c>
+      <c r="E9" t="n">
+        <v>19.17857142857143</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B10" t="n">
+        <v>91.65714285714286</v>
+      </c>
+      <c r="C10" t="n">
+        <v>75.42857142857143</v>
+      </c>
+      <c r="D10" t="n">
+        <v>35.64285714285715</v>
+      </c>
+      <c r="E10" t="n">
+        <v>19.21428571428572</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B11" t="n">
+        <v>91.09999999999999</v>
+      </c>
+      <c r="C11" t="n">
+        <v>75</v>
+      </c>
+      <c r="D11" t="n">
+        <v>35.75</v>
+      </c>
+      <c r="E11" t="n">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B12" t="n">
+        <v>90.54285714285714</v>
+      </c>
+      <c r="C12" t="n">
+        <v>74.57142857142857</v>
+      </c>
+      <c r="D12" t="n">
+        <v>35.85714285714285</v>
+      </c>
+      <c r="E12" t="n">
+        <v>19.28571428571428</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B13" t="n">
+        <v>89.98571428571429</v>
+      </c>
+      <c r="C13" t="n">
+        <v>74.14285714285714</v>
+      </c>
+      <c r="D13" t="n">
+        <v>35.96428571428572</v>
+      </c>
+      <c r="E13" t="n">
+        <v>19.32142857142857</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B14" t="n">
+        <v>89.42857142857143</v>
+      </c>
+      <c r="C14" t="n">
+        <v>73.71428571428571</v>
+      </c>
+      <c r="D14" t="n">
+        <v>36.07142857142857</v>
+      </c>
+      <c r="E14" t="n">
+        <v>19.35714285714286</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B15" t="n">
+        <v>88.87142857142857</v>
+      </c>
+      <c r="C15" t="n">
+        <v>73.28571428571429</v>
+      </c>
+      <c r="D15" t="n">
+        <v>36.17857142857143</v>
+      </c>
+      <c r="E15" t="n">
+        <v>19.39285714285714</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B16" t="n">
+        <v>88.31428571428572</v>
+      </c>
+      <c r="C16" t="n">
+        <v>72.85714285714286</v>
+      </c>
+      <c r="D16" t="n">
+        <v>36.28571428571428</v>
+      </c>
+      <c r="E16" t="n">
+        <v>19.42857142857143</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B17" t="n">
+        <v>87.75714285714287</v>
+      </c>
+      <c r="C17" t="n">
+        <v>72.42857142857143</v>
+      </c>
+      <c r="D17" t="n">
+        <v>36.39285714285715</v>
+      </c>
+      <c r="E17" t="n">
+        <v>19.46428571428572</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B18" t="n">
+        <v>87.2</v>
+      </c>
+      <c r="C18" t="n">
+        <v>72</v>
+      </c>
+      <c r="D18" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Source: Figure8_Cattle_Inventory.csv [S071], scaled series for LATAM/India.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
batch B: expand regulatory table and fix figure 6 sensitivity
</commit_message>
<xml_diff>
--- a/_figures/figures_data.xlsx
+++ b/_figures/figures_data.xlsx
@@ -20638,6 +20638,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -20684,14 +20685,14 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Price Sensitivity (Inv)</t>
+          <t>Price Sensitivity</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>8</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
batch D: upgrade appendix tables with flags/logo badges and add actor ecosystem figure
</commit_message>
<xml_diff>
--- a/_figures/figures_data.xlsx
+++ b/_figures/figures_data.xlsx
@@ -55,11 +55,11 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 46" sheetId="47" state="visible" r:id="rId47"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 47" sheetId="48" state="visible" r:id="rId48"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 48" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 49" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DOCX_TABLE_SYNC" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DOCX_FIGURE_HARMONIZATION" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 50" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure Cattle Inventory" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DOCX_TABLE_SYNC" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DOCX_FIGURE_HARMONIZATION" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 50" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure Cattle Inventory" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Figure 49" sheetId="54" state="visible" r:id="rId54"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -17210,221 +17210,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Revenue architecture across pharma-linked, feed-linked, and consumer-led models.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Estimated 2024 Revenue (USD Billions)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Segment</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Nestlé Purina</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>22.4</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Pet Food &amp; CPG</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Mars Petcare</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>22</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Pet Food &amp; CPG</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Hill's</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Pet Food &amp; CPG</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Blue Buffalo</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Pet Food &amp; CPG</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Zoetis</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Pharma &amp; Animal Health</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Merck AH</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Pharma &amp; Animal Health</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Boehringer Ingelheim</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>5</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Pharma &amp; Animal Health</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Elanco</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Pharma &amp; Animal Health</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>DSM-Firmenich</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Feed &amp; Specialty Inputs</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Novonesis</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Feed &amp; Specialty Inputs</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Phibro</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Feed &amp; Specialty Inputs</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Source: Zoetis 10-K [S115]; DSM-Firmenich Annual [S117]; Swedencare Annual [S118]; Virbac Annual [S119]; Dechra Annual [S120].</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17734,7 +17519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -19755,7 +19540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -19970,7 +19755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -20277,6 +20062,481 @@
       <c r="A20" t="inlineStr">
         <is>
           <t>Source: Figure8_Cattle_Inventory.csv [S071], scaled series for LATAM/India.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Actor Ecosystem by Strategic Group (Logo-based map)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Group</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Logo_Slug</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pharma / Animal Health</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Zoetis</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>zoetis</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pharma / Animal Health</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Elanco</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>elanco</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pharma / Animal Health</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dechra</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dechra</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Pharma / Animal Health</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Virbac</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>virbac</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Pharma / Animal Health</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Vetoquinol</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vetoquinol</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Pet Nutrition &amp; Retail</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mars Petcare</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>mars_petcare</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Pet Nutrition &amp; Retail</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Nestle Purina</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>nestle_purina</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pet Nutrition &amp; Retail</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Hill's</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>hill_s</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Pet Nutrition &amp; Retail</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Chewy</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>chewy</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Pet Nutrition &amp; Retail</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Petco</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>petco</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Feed &amp; Ingredient Tech</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DSM-Firmenich</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>dsm_firmenich</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Feed &amp; Ingredient Tech</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Novonesis</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>novonesis</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Feed &amp; Ingredient Tech</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Phibro</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>phibro</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Feed &amp; Ingredient Tech</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ADM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>adm</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Feed &amp; Ingredient Tech</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Evonik</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>evonik</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Nutraceutical Specialists</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Swedencare</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>swedencare</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Nutraceutical Specialists</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Nutramax</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>nutramax</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Nutraceutical Specialists</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FoodScience</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>foodscience</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Nutraceutical Specialists</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>YuMOVE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>yumove</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Nutraceutical Specialists</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>AnimalBiome</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>animalbiome</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Investor Platforms</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>EQT Group</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>eqt_group</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Investor Platforms</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Gryphon Investors</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>gryphon_investors</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Investor Platforms</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Cinven</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>cinven</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Investor Platforms</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Anterra Capital</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>anterra_capital</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Investor Platforms</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Aqua-Spark</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>aqua_spark</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Source: Internal platform mapping synthesis from Table B.1 and Table C.1</t>
         </is>
       </c>
     </row>
@@ -20638,7 +20898,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>

</xml_diff>